<commit_message>
updated model optimization attempt excel sheet
</commit_message>
<xml_diff>
--- a/Model_Notebook/Model_Optimization_Notes.xlsx
+++ b/Model_Notebook/Model_Optimization_Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukew\Documents\UofM_Data_Analytics_Coursework\Section5\project4_convolutional_nerual_networks\Obesity-Prediction-Model\Model_Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B4B00A-8049-4D28-8B0F-CE656FADF20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021EE2D7-AF80-424E-B255-0E5CD97E3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60120" yWindow="4515" windowWidth="21600" windowHeight="11235" xr2:uid="{3AD1EAFC-48E1-4F83-80B9-631E8F768C4B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Attempt ID</t>
   </si>
@@ -88,10 +88,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4F3A0A-6093-433A-BB4B-A5F9A9ABD20E}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,10 +589,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5">
-        <v>6289</v>
+        <v>2537</v>
       </c>
       <c r="E5">
         <v>8417</v>
@@ -592,8 +600,8 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>9.0807000000000002</v>
+      <c r="G5" t="s">
+        <v>9</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -601,8 +609,8 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="J5">
-        <v>0.83240000000000003</v>
+      <c r="J5" s="1">
+        <v>0.74570000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -625,19 +633,52 @@
         <v>10</v>
       </c>
       <c r="G6">
+        <v>9.0807000000000002</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>0.83240000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>87</v>
+      </c>
+      <c r="D7">
+        <v>6289</v>
+      </c>
+      <c r="E7">
+        <v>8417</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
         <v>8.7318999999999996</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>7.1962999999999999</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>2.9550000000000001</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>0.83120000000000005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated notebooks and model trial data
</commit_message>
<xml_diff>
--- a/Model_Notebook/Model_Optimization_Notes.xlsx
+++ b/Model_Notebook/Model_Optimization_Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukew\Documents\UofM_Data_Analytics_Coursework\Section5\project4_convolutional_nerual_networks\Obesity-Prediction-Model\Model_Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021EE2D7-AF80-424E-B255-0E5CD97E3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAD37C3-5B98-4F2F-90E8-686A2EAC41F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60120" yWindow="4515" windowWidth="21600" windowHeight="11235" xr2:uid="{3AD1EAFC-48E1-4F83-80B9-631E8F768C4B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11175" xr2:uid="{3AD1EAFC-48E1-4F83-80B9-631E8F768C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t>Attempt ID</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Loss Function</t>
+  </si>
+  <si>
+    <t>linear regression</t>
+  </si>
+  <si>
+    <t>random forest regressor</t>
+  </si>
+  <si>
+    <t>n_estimators</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4F3A0A-6093-433A-BB4B-A5F9A9ABD20E}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +462,7 @@
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,22 +479,25 @@
         <v>12</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -501,23 +513,23 @@
       <c r="E2">
         <v>6025</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -533,23 +545,23 @@
       <c r="E3">
         <v>6025</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2.6320000000000001</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" t="s">
         <v>9</v>
       </c>
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -565,23 +577,23 @@
       <c r="E4">
         <v>8113</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
         <v>15.17</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
       <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -597,11 +609,8 @@
       <c r="E5">
         <v>8417</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -609,11 +618,14 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.74570000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -629,23 +641,23 @@
       <c r="E6">
         <v>8417</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
         <v>9.0807000000000002</v>
       </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
       <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6">
         <v>0.83240000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -661,20 +673,227 @@
       <c r="E7">
         <v>8417</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
         <v>8.7318999999999996</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>7.1962999999999999</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2.9550000000000001</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.83120000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>6289</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>14.943</v>
+      </c>
+      <c r="I8">
+        <v>7.6946000000000003</v>
+      </c>
+      <c r="J8">
+        <v>3.8656000000000001</v>
+      </c>
+      <c r="K8">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="D9">
+        <v>6289</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>13.444100000000001</v>
+      </c>
+      <c r="I9">
+        <v>7.2004999999999999</v>
+      </c>
+      <c r="J9">
+        <v>3.6665999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.74039999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>87</v>
+      </c>
+      <c r="D10">
+        <v>6289</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>12.8613</v>
+      </c>
+      <c r="I10">
+        <v>7.2004999999999999</v>
+      </c>
+      <c r="J10">
+        <v>3.5861999999999998</v>
+      </c>
+      <c r="K10">
+        <v>0.75170000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>6289</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>12.736499999999999</v>
+      </c>
+      <c r="I11">
+        <v>7.2004999999999999</v>
+      </c>
+      <c r="J11">
+        <v>3.5688</v>
+      </c>
+      <c r="K11">
+        <v>0.75409999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>87</v>
+      </c>
+      <c r="D12">
+        <v>6289</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>250</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>12.692399999999999</v>
+      </c>
+      <c r="I12">
+        <v>7.2004999999999999</v>
+      </c>
+      <c r="J12">
+        <v>3.5626000000000002</v>
+      </c>
+      <c r="K12">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>87</v>
+      </c>
+      <c r="D13">
+        <v>6289</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>1000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>12.6256</v>
+      </c>
+      <c r="I13">
+        <v>7.2004999999999999</v>
+      </c>
+      <c r="J13">
+        <v>3.5529999999999999</v>
+      </c>
+      <c r="K13">
+        <v>0.75619999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>